<commit_message>
add plate and pole
</commit_message>
<xml_diff>
--- a/発注リスト07_29.xlsx
+++ b/発注リスト07_29.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hibik\Desktop\ロボメカ\Rescue\2年\子機_本選\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD42067-AAFE-4D44-832C-8379153105E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117A70BC-FC4F-43DF-B750-95625FD7BAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BF0F75F-CDC4-48A2-A6F4-864072C7B257}"/>
   </bookViews>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1012,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8DD0AE-6BA2-498D-AEB5-0A7E6DCCC7CB}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="109" workbookViewId="0">
+      <selection activeCell="Q65" sqref="Q65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>